<commit_message>
updated results and conclusion
</commit_message>
<xml_diff>
--- a/allResults/StrategyResults.xlsx
+++ b/allResults/StrategyResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/908232a7ec8e8e09/Desktop/algo_trading_and_ML/allResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{23284190-1528-49D5-800F-1AB334F958E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AF34F6-5E64-4A62-9A1C-C197D63CFE59}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{23284190-1528-49D5-800F-1AB334F958E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B7C1A3-5601-4B35-8CAD-7628490347B9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3435" windowWidth="29040" windowHeight="15720" xr2:uid="{E9BBB7AA-608A-4F59-93B8-BC2B29940EB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>Assets</t>
   </si>
@@ -110,13 +110,37 @@
   </si>
   <si>
     <t>Nov-18 - Oct-22</t>
+  </si>
+  <si>
+    <t>Sharpe Ratios</t>
+  </si>
+  <si>
+    <t>RF (normalized)</t>
+  </si>
+  <si>
+    <t>ML &amp; ANN</t>
+  </si>
+  <si>
+    <t>Established</t>
+  </si>
+  <si>
+    <t>RF (standard)</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>Returns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +171,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +210,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -297,11 +346,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -344,11 +405,29 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -356,44 +435,99 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,71 +844,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FDA801-551B-4DA6-94AB-AD56F8094497}">
-  <dimension ref="B2:K11"/>
+  <dimension ref="B2:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.88671875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.21875" style="7" customWidth="1"/>
     <col min="8" max="8" width="4.109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" style="6" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="6"/>
+    <col min="13" max="13" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="2:11" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="29"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="21"/>
+      <c r="J2" s="39"/>
+      <c r="M2" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="21"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="27"/>
       <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="31"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M3" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -795,12 +945,21 @@
       <c r="I4" s="10">
         <v>0.69589999999999996</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M4" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="59">
+        <v>0</v>
+      </c>
+      <c r="O4" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -821,11 +980,20 @@
       <c r="I5" s="10">
         <v>0.12809999999999999</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="51">
+        <v>3</v>
+      </c>
+      <c r="O5" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -835,22 +1003,31 @@
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="9">
         <v>0.14949999999999999</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="16">
         <v>1.84E-2</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="51">
+        <v>2</v>
+      </c>
+      <c r="O6" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -860,22 +1037,31 @@
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="16">
         <v>7.4700000000000003E-2</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="9">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M7" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="59">
+        <v>0</v>
+      </c>
+      <c r="O7" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -885,22 +1071,25 @@
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="9">
         <v>0.23080000000000001</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="9">
         <v>0.16739999999999999</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M8" s="52"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="54"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -910,22 +1099,27 @@
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="9">
         <v>0.13569999999999999</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="9">
         <v>0.13170000000000001</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M9" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="57"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -935,22 +1129,31 @@
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="10">
         <v>6.3500000000000001E-2</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="10">
         <v>4.8599999999999997E-2</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M10" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="59">
+        <v>0</v>
+      </c>
+      <c r="O10" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -960,23 +1163,407 @@
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="9">
         <v>6.6400000000000001E-2</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="17">
         <v>4.24E-2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="M11" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="51">
+        <v>1</v>
+      </c>
+      <c r="O11" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M12" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="51">
+        <v>2</v>
+      </c>
+      <c r="O12" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M13" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="59">
+        <v>0</v>
+      </c>
+      <c r="O13" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="37"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="39"/>
+      <c r="M17" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="35"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="56"/>
+      <c r="O18" s="57"/>
+    </row>
+    <row r="19" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="41">
+        <v>-0.38</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="42">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="42">
+        <v>0.77</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="59">
+        <v>0</v>
+      </c>
+      <c r="O19" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="41">
+        <v>0.61</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="42">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="51">
+        <v>3</v>
+      </c>
+      <c r="O20" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="43">
+        <v>0.22</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="51">
+        <v>2</v>
+      </c>
+      <c r="O21" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0.43</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="44">
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="43">
+        <v>0.38</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="59">
+        <v>0</v>
+      </c>
+      <c r="O22" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="41">
+        <v>0.16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="43">
+        <v>0.76</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="43">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="52"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="54"/>
+    </row>
+    <row r="24" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="41">
+        <v>0.38</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="43">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="I24" s="43">
+        <v>0.53</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" s="56"/>
+      <c r="O24" s="57"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="41">
+        <v>0.35</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="42">
+        <v>0.54</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="42">
+        <v>0.38</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" s="59">
+        <v>0</v>
+      </c>
+      <c r="O25" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="41">
+        <v>-0.62</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="43">
+        <v>0.81</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="51">
+        <v>1</v>
+      </c>
+      <c r="O26" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M27" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" s="51">
+        <v>2</v>
+      </c>
+      <c r="O27" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M28" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" s="59">
+        <v>0</v>
+      </c>
+      <c r="O28" s="51">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="24">
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="H21:H26"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="H2:H3"/>

</xml_diff>